<commit_message>
updated to latest olo
</commit_message>
<xml_diff>
--- a/src/module1/KWD-loginGmail.xlsx
+++ b/src/module1/KWD-loginGmail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
     <t>login.password</t>
   </si>
   <si>
-    <t>&lt;&lt;username&gt;&gt;</t>
-  </si>
-  <si>
-    <t>&lt;&lt;password&gt;&gt;</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>password2</t>
+  </si>
+  <si>
+    <t>{{username}}</t>
+  </si>
+  <si>
+    <t>{{password}}</t>
   </si>
 </sst>
 </file>
@@ -446,9 +446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -493,26 +493,26 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -527,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -537,26 +537,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>